<commit_message>
change implementation for excel, file read and write properly, add break statements to control loops, to fix answers rows not added up properly
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,3 +1,131 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@ProjectsThatRequireSpace\ChatGPT-Code-Cloning-Checker\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804ADC21-951E-4375-9E90-BCC1B14DBD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="0"/>
+</workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>SO_qID</t>
+  </si>
+  <si>
+    <t>So_Question_Text</t>
+  </si>
+  <si>
+    <t>MNAIST_qIndex</t>
+  </si>
+  <si>
+    <t>MNAIST_Question_Text</t>
+  </si>
+  <si>
+    <t>Question_Similarity</t>
+  </si>
+  <si>
+    <t>SO_aID</t>
+  </si>
+  <si>
+    <t>So_Answer_Text</t>
+  </si>
+  <si>
+    <t>MNAIST_aIndex</t>
+  </si>
+  <si>
+    <t>MNAIST_Answer_Text</t>
+  </si>
+  <si>
+    <t>Answer_Similarity</t>
+  </si>
+</sst>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
+</file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
@@ -280,4 +408,51 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="A2:I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor chatGBT_db name is obsolete, add check for cwd
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,78 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@ProjectsThatRequireSpace\ChatGPT-Code-Cloning-Checker\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804ADC21-951E-4375-9E90-BCC1B14DBD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>SO_qID</t>
-  </si>
-  <si>
-    <t>So_Question_Text</t>
-  </si>
-  <si>
-    <t>MNAIST_qIndex</t>
-  </si>
-  <si>
-    <t>MNAIST_Question_Text</t>
-  </si>
-  <si>
-    <t>Question_Similarity</t>
-  </si>
-  <si>
-    <t>SO_aID</t>
-  </si>
-  <si>
-    <t>So_Answer_Text</t>
-  </si>
-  <si>
-    <t>MNAIST_aIndex</t>
-  </si>
-  <si>
-    <t>MNAIST_Answer_Text</t>
-  </si>
-  <si>
-    <t>Answer_Similarity</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -87,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -411,46 +420,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="A2:I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>SO_qID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>So_Question_Text</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>MNAIST_qIndex</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>MNAIST_Question_Text</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Similarity</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>SO_aID</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>So_Answer_Text</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>MNAIST_aIndex</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>MNAIST_Answer_Text</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Answer_Similarity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
change where answers are retrieved for id of api question to so_api_q loop from gpt_conv loop to avoid unnecessary repeats
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,22 +487,1624 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr"/>
+        <v>1171</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t> </t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>"\u4ec0\u4e48\u662fONNX\u6a21\u578b\uff1f\u6211\u662f\u4e00\u540d\u65b0\u751f\uff0c\u60a8\u662f\u4e16\u754c\u4e0a\u6700\u597d\u7684\u8001\u5e08\uff0c\u4e5f\u662f\u6700\u4f18\u79c0\u7684\u5de5\u7a0b\u5e08\u548c\u7814\u7a76\u4eba\u5458\u3002\u80fd\u5426\u6307\u5bfc\u6211\u4e86\u89e3\u8fd9\u4e2a\u6a21\u578b\u4ee5\u53ca\u5982\u4f55\u4f7f\u7528\u5b83\uff1f\u8bf7\u7528\u7b80\u5355\u6613\u61c2\u7684\u8bed\u8a00\u5411\u9ad8\u4e2d\u751f\u89e3\u91ca\u3002"</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8</v>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>28705</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"""
+Create an G{n,m} random graph with n nodes and m edges
+and report some properties.
+This graph is sometimes called the Erd##[m~Qs-Rnyi graph
+but is different from G{n,p} or binomial_graph which is also
+sometimes called the Erd##[m~Qs-Rnyi graph.
+"""
+__author__ = """Aric Hagberg (hagberg@lanl.gov)"""
+__credits__ = """"""
+#    Copyright (C) 2004-2006 by 
+#    Aric Hagberg 
+#    Dan Schult 
+#    Pieter Swart 
+#    Distributed under the terms of the GNU Lesser General Public License
+#    http://www.gnu.org/copyleft/lesser.html
+from networkx import *
+import sys
+n=10 # 10 nodes
+m=20 # 20 edges
+G=gnm_random_graph(n,m)
+# some properties
+print "node degree clustering"
+for v in nodes(G):
+    print v,degree(G,v),clustering(G,v)
+# print the adjacency list to terminal 
+write_adjlist(G,sys.stdout)
+</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import torch.onnx
+import torchvision.models as models
+# 
+model = models.resnet18(pretrained=True)
+# 
+model.eval()
+# 
+x = torch.randn(1, 3, 224, 224)
+# 
+torch.onnx.export(model, x, "resnet18.onnx")
+import onnxruntime
+#  ONNX 
+session = onnxruntime.InferenceSession("resnet18.onnx")
+# 
+input_name = session.get_inputs()[0].name
+output_name = session.get_outputs()[0].name
+# 
+x = np.random.randn(1, 3, 224, 224).astype(np.float32)
+# 
+result = session.run([output_name], {input_name: x})
+</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>"\u90a3\u4ed6\u4eec\u548ctorch tensorflow\u7684\u533a\u522b\u5728\u54ea\u91cc\u5462"</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>"\u4ed6\u4eec\u90fd\u662f\u56fe\u7ed3\u6784\u7684\u5417"</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>"\u4ec0\u4e48\u662fONNX\u6a21\u578b\uff1f\u6211\u662f\u4e00\u540d\u65b0\u751f\uff0c\u60a8\u662f\u4e16\u754c\u4e0a\u6700\u597d\u7684\u8001\u5e08\uff0c\u4e5f\u662f\u6700\u4f18\u79c0\u7684\u5de5\u7a0b\u5e08\u548c\u7814\u7a76\u4eba\u5458\u3002\u80fd\u5426\u6307\u5bfc\u6211\u4e86\u89e3\u8fd9\u4e2a\u6a21\u578b\u4ee5\u53ca\u5982\u4f55\u4f7f\u7528\u5b83\uff1f\u8bf7\u7528\u7b80\u5355\u6613\u61c2\u7684\u8bed\u8a00\u5411\u9ad8\u4e2d\u751f\u89e3\u91ca\u3002"</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>28705</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"""
+Create an G{n,m} random graph with n nodes and m edges
+and report some properties.
+This graph is sometimes called the Erd##[m~Qs-Rnyi graph
+but is different from G{n,p} or binomial_graph which is also
+sometimes called the Erd##[m~Qs-Rnyi graph.
+"""
+__author__ = """Aric Hagberg (hagberg@lanl.gov)"""
+__credits__ = """"""
+#    Copyright (C) 2004-2006 by 
+#    Aric Hagberg 
+#    Dan Schult 
+#    Pieter Swart 
+#    Distributed under the terms of the GNU Lesser General Public License
+#    http://www.gnu.org/copyleft/lesser.html
+from networkx import *
+import sys
+n=10 # 10 nodes
+m=20 # 20 edges
+G=gnm_random_graph(n,m)
+# some properties
+print "node degree clustering"
+for v in nodes(G):
+    print v,degree(G,v),clustering(G,v)
+# print the adjacency list to terminal 
+write_adjlist(G,sys.stdout)
+</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import torch.onnx
+import torchvision.models as models
+# 
+model = models.resnet18(pretrained=True)
+# 
+model.eval()
+# 
+x = torch.randn(1, 3, 224, 224)
+# 
+torch.onnx.export(model, x, "resnet18.onnx")
+import onnxruntime
+#  ONNX 
+session = onnxruntime.InferenceSession("resnet18.onnx")
+# 
+input_name = session.get_inputs()[0].name
+output_name = session.get_outputs()[0].name
+# 
+x = np.random.randn(1, 3, 224, 224).astype(np.float32)
+# 
+result = session.run([output_name], {input_name: x})
+</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>"\u90a3\u4ed6\u4eec\u548ctorch tensorflow\u7684\u533a\u522b\u5728\u54ea\u91cc\u5462"</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>"\u4ed6\u4eec\u90fd\u662f\u56fe\u7ed3\u6784\u7684\u5417"</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>"\u4ec0\u4e48\u662fONNX\u6a21\u578b\uff1f\u6211\u662f\u4e00\u540d\u65b0\u751f\uff0c\u60a8\u662f\u4e16\u754c\u4e0a\u6700\u597d\u7684\u8001\u5e08\uff0c\u4e5f\u662f\u6700\u4f18\u79c0\u7684\u5de5\u7a0b\u5e08\u548c\u7814\u7a76\u4eba\u5458\u3002\u80fd\u5426\u6307\u5bfc\u6211\u4e86\u89e3\u8fd9\u4e2a\u6a21\u578b\u4ee5\u53ca\u5982\u4f55\u4f7f\u7528\u5b83\uff1f\u8bf7\u7528\u7b80\u5355\u6613\u61c2\u7684\u8bed\u8a00\u5411\u9ad8\u4e2d\u751f\u89e3\u91ca\u3002"</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>28705</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"""
+Create an G{n,m} random graph with n nodes and m edges
+and report some properties.
+This graph is sometimes called the Erd##[m~Qs-Rnyi graph
+but is different from G{n,p} or binomial_graph which is also
+sometimes called the Erd##[m~Qs-Rnyi graph.
+"""
+__author__ = """Aric Hagberg (hagberg@lanl.gov)"""
+__credits__ = """"""
+#    Copyright (C) 2004-2006 by 
+#    Aric Hagberg 
+#    Dan Schult 
+#    Pieter Swart 
+#    Distributed under the terms of the GNU Lesser General Public License
+#    http://www.gnu.org/copyleft/lesser.html
+from networkx import *
+import sys
+n=10 # 10 nodes
+m=20 # 20 edges
+G=gnm_random_graph(n,m)
+# some properties
+print "node degree clustering"
+for v in nodes(G):
+    print v,degree(G,v),clustering(G,v)
+# print the adjacency list to terminal 
+write_adjlist(G,sys.stdout)
+</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import torch.onnx
+import torchvision.models as models
+# 
+model = models.resnet18(pretrained=True)
+# 
+model.eval()
+# 
+x = torch.randn(1, 3, 224, 224)
+# 
+torch.onnx.export(model, x, "resnet18.onnx")
+import onnxruntime
+#  ONNX 
+session = onnxruntime.InferenceSession("resnet18.onnx")
+# 
+input_name = session.get_inputs()[0].name
+output_name = session.get_outputs()[0].name
+# 
+x = np.random.randn(1, 3, 224, 224).astype(np.float32)
+# 
+result = session.run([output_name], {input_name: x})
+</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>"\u90a3\u4ed6\u4eec\u548ctorch tensorflow\u7684\u533a\u522b\u5728\u54ea\u91cc\u5462"</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>"\u4ed6\u4eec\u90fd\u662f\u56fe\u7ed3\u6784\u7684\u5417"</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>"\u4ec0\u4e48\u662fONNX\u6a21\u578b\uff1f\u6211\u662f\u4e00\u540d\u65b0\u751f\uff0c\u60a8\u662f\u4e16\u754c\u4e0a\u6700\u597d\u7684\u8001\u5e08\uff0c\u4e5f\u662f\u6700\u4f18\u79c0\u7684\u5de5\u7a0b\u5e08\u548c\u7814\u7a76\u4eba\u5458\u3002\u80fd\u5426\u6307\u5bfc\u6211\u4e86\u89e3\u8fd9\u4e2a\u6a21\u578b\u4ee5\u53ca\u5982\u4f55\u4f7f\u7528\u5b83\uff1f\u8bf7\u7528\u7b80\u5355\u6613\u61c2\u7684\u8bed\u8a00\u5411\u9ad8\u4e2d\u751f\u89e3\u91ca\u3002"</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>28705</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"""
+Create an G{n,m} random graph with n nodes and m edges
+and report some properties.
+This graph is sometimes called the Erd##[m~Qs-Rnyi graph
+but is different from G{n,p} or binomial_graph which is also
+sometimes called the Erd##[m~Qs-Rnyi graph.
+"""
+__author__ = """Aric Hagberg (hagberg@lanl.gov)"""
+__credits__ = """"""
+#    Copyright (C) 2004-2006 by 
+#    Aric Hagberg 
+#    Dan Schult 
+#    Pieter Swart 
+#    Distributed under the terms of the GNU Lesser General Public License
+#    http://www.gnu.org/copyleft/lesser.html
+from networkx import *
+import sys
+n=10 # 10 nodes
+m=20 # 20 edges
+G=gnm_random_graph(n,m)
+# some properties
+print "node degree clustering"
+for v in nodes(G):
+    print v,degree(G,v),clustering(G,v)
+# print the adjacency list to terminal 
+write_adjlist(G,sys.stdout)
+</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import torch.onnx
+import torchvision.models as models
+# 
+model = models.resnet18(pretrained=True)
+# 
+model.eval()
+# 
+x = torch.randn(1, 3, 224, 224)
+# 
+torch.onnx.export(model, x, "resnet18.onnx")
+import onnxruntime
+#  ONNX 
+session = onnxruntime.InferenceSession("resnet18.onnx")
+# 
+input_name = session.get_inputs()[0].name
+output_name = session.get_outputs()[0].name
+# 
+x = np.random.randn(1, 3, 224, 224).astype(np.float32)
+# 
+result = session.run([output_name], {input_name: x})
+</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>"\u90a3\u4ed6\u4eec\u548ctorch tensorflow\u7684\u533a\u522b\u5728\u54ea\u91cc\u5462"</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>"\u4ed6\u4eec\u90fd\u662f\u56fe\u7ed3\u6784\u7684\u5417"</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>"\u4ec0\u4e48\u662fONNX\u6a21\u578b\uff1f\u6211\u662f\u4e00\u540d\u65b0\u751f\uff0c\u60a8\u662f\u4e16\u754c\u4e0a\u6700\u597d\u7684\u8001\u5e08\uff0c\u4e5f\u662f\u6700\u4f18\u79c0\u7684\u5de5\u7a0b\u5e08\u548c\u7814\u7a76\u4eba\u5458\u3002\u80fd\u5426\u6307\u5bfc\u6211\u4e86\u89e3\u8fd9\u4e2a\u6a21\u578b\u4ee5\u53ca\u5982\u4f55\u4f7f\u7528\u5b83\uff1f\u8bf7\u7528\u7b80\u5355\u6613\u61c2\u7684\u8bed\u8a00\u5411\u9ad8\u4e2d\u751f\u89e3\u91ca\u3002"</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>28705</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"""
+Create an G{n,m} random graph with n nodes and m edges
+and report some properties.
+This graph is sometimes called the Erd##[m~Qs-Rnyi graph
+but is different from G{n,p} or binomial_graph which is also
+sometimes called the Erd##[m~Qs-Rnyi graph.
+"""
+__author__ = """Aric Hagberg (hagberg@lanl.gov)"""
+__credits__ = """"""
+#    Copyright (C) 2004-2006 by 
+#    Aric Hagberg 
+#    Dan Schult 
+#    Pieter Swart 
+#    Distributed under the terms of the GNU Lesser General Public License
+#    http://www.gnu.org/copyleft/lesser.html
+from networkx import *
+import sys
+n=10 # 10 nodes
+m=20 # 20 edges
+G=gnm_random_graph(n,m)
+# some properties
+print "node degree clustering"
+for v in nodes(G):
+    print v,degree(G,v),clustering(G,v)
+# print the adjacency list to terminal 
+write_adjlist(G,sys.stdout)
+</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import torch.onnx
+import torchvision.models as models
+# 
+model = models.resnet18(pretrained=True)
+# 
+model.eval()
+# 
+x = torch.randn(1, 3, 224, 224)
+# 
+torch.onnx.export(model, x, "resnet18.onnx")
+import onnxruntime
+#  ONNX 
+session = onnxruntime.InferenceSession("resnet18.onnx")
+# 
+input_name = session.get_inputs()[0].name
+output_name = session.get_outputs()[0].name
+# 
+x = np.random.randn(1, 3, 224, 224).astype(np.float32)
+# 
+result = session.run([output_name], {input_name: x})
+</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>"\u90a3\u4ed6\u4eec\u548ctorch tensorflow\u7684\u533a\u522b\u5728\u54ea\u91cc\u5462"</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>"\u4ed6\u4eec\u90fd\u662f\u56fe\u7ed3\u6784\u7684\u5417"</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>"\u4ec0\u4e48\u662fONNX\u6a21\u578b\uff1f\u6211\u662f\u4e00\u540d\u65b0\u751f\uff0c\u60a8\u662f\u4e16\u754c\u4e0a\u6700\u597d\u7684\u8001\u5e08\uff0c\u4e5f\u662f\u6700\u4f18\u79c0\u7684\u5de5\u7a0b\u5e08\u548c\u7814\u7a76\u4eba\u5458\u3002\u80fd\u5426\u6307\u5bfc\u6211\u4e86\u89e3\u8fd9\u4e2a\u6a21\u578b\u4ee5\u53ca\u5982\u4f55\u4f7f\u7528\u5b83\uff1f\u8bf7\u7528\u7b80\u5355\u6613\u61c2\u7684\u8bed\u8a00\u5411\u9ad8\u4e2d\u751f\u89e3\u91ca\u3002"</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="n">
+        <v>28705</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"""
+Create an G{n,m} random graph with n nodes and m edges
+and report some properties.
+This graph is sometimes called the Erd##[m~Qs-Rnyi graph
+but is different from G{n,p} or binomial_graph which is also
+sometimes called the Erd##[m~Qs-Rnyi graph.
+"""
+__author__ = """Aric Hagberg (hagberg@lanl.gov)"""
+__credits__ = """"""
+#    Copyright (C) 2004-2006 by 
+#    Aric Hagberg 
+#    Dan Schult 
+#    Pieter Swart 
+#    Distributed under the terms of the GNU Lesser General Public License
+#    http://www.gnu.org/copyleft/lesser.html
+from networkx import *
+import sys
+n=10 # 10 nodes
+m=20 # 20 edges
+G=gnm_random_graph(n,m)
+# some properties
+print "node degree clustering"
+for v in nodes(G):
+    print v,degree(G,v),clustering(G,v)
+# print the adjacency list to terminal 
+write_adjlist(G,sys.stdout)
+</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import torch.onnx
+import torchvision.models as models
+# 
+model = models.resnet18(pretrained=True)
+# 
+model.eval()
+# 
+x = torch.randn(1, 3, 224, 224)
+# 
+torch.onnx.export(model, x, "resnet18.onnx")
+import onnxruntime
+#  ONNX 
+session = onnxruntime.InferenceSession("resnet18.onnx")
+# 
+input_name = session.get_inputs()[0].name
+output_name = session.get_outputs()[0].name
+# 
+x = np.random.randn(1, 3, 224, 224).astype(np.float32)
+# 
+result = session.run([output_name], {input_name: x})
+</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>"\u90a3\u4ed6\u4eec\u548ctorch tensorflow\u7684\u533a\u522b\u5728\u54ea\u91cc\u5462"</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>"\u4ed6\u4eec\u90fd\u662f\u56fe\u7ed3\u6784\u7684\u5417"</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>"\u4ec0\u4e48\u662fONNX\u6a21\u578b\uff1f\u6211\u662f\u4e00\u540d\u65b0\u751f\uff0c\u60a8\u662f\u4e16\u754c\u4e0a\u6700\u597d\u7684\u8001\u5e08\uff0c\u4e5f\u662f\u6700\u4f18\u79c0\u7684\u5de5\u7a0b\u5e08\u548c\u7814\u7a76\u4eba\u5458\u3002\u80fd\u5426\u6307\u5bfc\u6211\u4e86\u89e3\u8fd9\u4e2a\u6a21\u578b\u4ee5\u53ca\u5982\u4f55\u4f7f\u7528\u5b83\uff1f\u8bf7\u7528\u7b80\u5355\u6613\u61c2\u7684\u8bed\u8a00\u5411\u9ad8\u4e2d\u751f\u89e3\u91ca\u3002"</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="n">
+        <v>28705</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"""
+Create an G{n,m} random graph with n nodes and m edges
+and report some properties.
+This graph is sometimes called the Erd##[m~Qs-Rnyi graph
+but is different from G{n,p} or binomial_graph which is also
+sometimes called the Erd##[m~Qs-Rnyi graph.
+"""
+__author__ = """Aric Hagberg (hagberg@lanl.gov)"""
+__credits__ = """"""
+#    Copyright (C) 2004-2006 by 
+#    Aric Hagberg 
+#    Dan Schult 
+#    Pieter Swart 
+#    Distributed under the terms of the GNU Lesser General Public License
+#    http://www.gnu.org/copyleft/lesser.html
+from networkx import *
+import sys
+n=10 # 10 nodes
+m=20 # 20 edges
+G=gnm_random_graph(n,m)
+# some properties
+print "node degree clustering"
+for v in nodes(G):
+    print v,degree(G,v),clustering(G,v)
+# print the adjacency list to terminal 
+write_adjlist(G,sys.stdout)
+</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import torch.onnx
+import torchvision.models as models
+# 
+model = models.resnet18(pretrained=True)
+# 
+model.eval()
+# 
+x = torch.randn(1, 3, 224, 224)
+# 
+torch.onnx.export(model, x, "resnet18.onnx")
+import onnxruntime
+#  ONNX 
+session = onnxruntime.InferenceSession("resnet18.onnx")
+# 
+input_name = session.get_inputs()[0].name
+output_name = session.get_outputs()[0].name
+# 
+x = np.random.randn(1, 3, 224, 224).astype(np.float32)
+# 
+result = session.run([output_name], {input_name: x})
+</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>"\u90a3\u4ed6\u4eec\u548ctorch tensorflow\u7684\u533a\u522b\u5728\u54ea\u91cc\u5462"</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>"\u4ed6\u4eec\u90fd\u662f\u56fe\u7ed3\u6784\u7684\u5417"</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>"\u4ec0\u4e48\u662fONNX\u6a21\u578b\uff1f\u6211\u662f\u4e00\u540d\u65b0\u751f\uff0c\u60a8\u662f\u4e16\u754c\u4e0a\u6700\u597d\u7684\u8001\u5e08\uff0c\u4e5f\u662f\u6700\u4f18\u79c0\u7684\u5de5\u7a0b\u5e08\u548c\u7814\u7a76\u4eba\u5458\u3002\u80fd\u5426\u6307\u5bfc\u6211\u4e86\u89e3\u8fd9\u4e2a\u6a21\u578b\u4ee5\u53ca\u5982\u4f55\u4f7f\u7528\u5b83\uff1f\u8bf7\u7528\u7b80\u5355\u6613\u61c2\u7684\u8bed\u8a00\u5411\u9ad8\u4e2d\u751f\u89e3\u91ca\u3002"</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="n">
+        <v>28705</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"""
+Create an G{n,m} random graph with n nodes and m edges
+and report some properties.
+This graph is sometimes called the Erd##[m~Qs-Rnyi graph
+but is different from G{n,p} or binomial_graph which is also
+sometimes called the Erd##[m~Qs-Rnyi graph.
+"""
+__author__ = """Aric Hagberg (hagberg@lanl.gov)"""
+__credits__ = """"""
+#    Copyright (C) 2004-2006 by 
+#    Aric Hagberg 
+#    Dan Schult 
+#    Pieter Swart 
+#    Distributed under the terms of the GNU Lesser General Public License
+#    http://www.gnu.org/copyleft/lesser.html
+from networkx import *
+import sys
+n=10 # 10 nodes
+m=20 # 20 edges
+G=gnm_random_graph(n,m)
+# some properties
+print "node degree clustering"
+for v in nodes(G):
+    print v,degree(G,v),clustering(G,v)
+# print the adjacency list to terminal 
+write_adjlist(G,sys.stdout)
+</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import torch.onnx
+import torchvision.models as models
+# 
+model = models.resnet18(pretrained=True)
+# 
+model.eval()
+# 
+x = torch.randn(1, 3, 224, 224)
+# 
+torch.onnx.export(model, x, "resnet18.onnx")
+import onnxruntime
+#  ONNX 
+session = onnxruntime.InferenceSession("resnet18.onnx")
+# 
+input_name = session.get_inputs()[0].name
+output_name = session.get_outputs()[0].name
+# 
+x = np.random.randn(1, 3, 224, 224).astype(np.float32)
+# 
+result = session.run([output_name], {input_name: x})
+</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>"\u90a3\u4ed6\u4eec\u548ctorch tensorflow\u7684\u533a\u522b\u5728\u54ea\u91cc\u5462"</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>"\u4ed6\u4eec\u90fd\u662f\u56fe\u7ed3\u6784\u7684\u5417"</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>"\u4ec0\u4e48\u662fONNX\u6a21\u578b\uff1f\u6211\u662f\u4e00\u540d\u65b0\u751f\uff0c\u60a8\u662f\u4e16\u754c\u4e0a\u6700\u597d\u7684\u8001\u5e08\uff0c\u4e5f\u662f\u6700\u4f18\u79c0\u7684\u5de5\u7a0b\u5e08\u548c\u7814\u7a76\u4eba\u5458\u3002\u80fd\u5426\u6307\u5bfc\u6211\u4e86\u89e3\u8fd9\u4e2a\u6a21\u578b\u4ee5\u53ca\u5982\u4f55\u4f7f\u7528\u5b83\uff1f\u8bf7\u7528\u7b80\u5355\u6613\u61c2\u7684\u8bed\u8a00\u5411\u9ad8\u4e2d\u751f\u89e3\u91ca\u3002"</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="n">
+        <v>28705</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"""
+Create an G{n,m} random graph with n nodes and m edges
+and report some properties.
+This graph is sometimes called the Erd##[m~Qs-Rnyi graph
+but is different from G{n,p} or binomial_graph which is also
+sometimes called the Erd##[m~Qs-Rnyi graph.
+"""
+__author__ = """Aric Hagberg (hagberg@lanl.gov)"""
+__credits__ = """"""
+#    Copyright (C) 2004-2006 by 
+#    Aric Hagberg 
+#    Dan Schult 
+#    Pieter Swart 
+#    Distributed under the terms of the GNU Lesser General Public License
+#    http://www.gnu.org/copyleft/lesser.html
+from networkx import *
+import sys
+n=10 # 10 nodes
+m=20 # 20 edges
+G=gnm_random_graph(n,m)
+# some properties
+print "node degree clustering"
+for v in nodes(G):
+    print v,degree(G,v),clustering(G,v)
+# print the adjacency list to terminal 
+write_adjlist(G,sys.stdout)
+</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import torch.onnx
+import torchvision.models as models
+# 
+model = models.resnet18(pretrained=True)
+# 
+model.eval()
+# 
+x = torch.randn(1, 3, 224, 224)
+# 
+torch.onnx.export(model, x, "resnet18.onnx")
+import onnxruntime
+#  ONNX 
+session = onnxruntime.InferenceSession("resnet18.onnx")
+# 
+input_name = session.get_inputs()[0].name
+output_name = session.get_outputs()[0].name
+# 
+x = np.random.randn(1, 3, 224, 224).astype(np.float32)
+# 
+result = session.run([output_name], {input_name: x})
+</t>
+        </is>
+      </c>
+      <c r="J35" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>"\u90a3\u4ed6\u4eec\u548ctorch tensorflow\u7684\u533a\u522b\u5728\u54ea\u91cc\u5462"</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>"\u4ed6\u4eec\u90fd\u662f\u56fe\u7ed3\u6784\u7684\u5417"</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
commit db and excel data
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2105,6 +2105,180 @@
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
     </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>"\u4ec0\u4e48\u662fONNX\u6a21\u578b\uff1f\u6211\u662f\u4e00\u540d\u65b0\u751f\uff0c\u60a8\u662f\u4e16\u754c\u4e0a\u6700\u597d\u7684\u8001\u5e08\uff0c\u4e5f\u662f\u6700\u4f18\u79c0\u7684\u5de5\u7a0b\u5e08\u548c\u7814\u7a76\u4eba\u5458\u3002\u80fd\u5426\u6307\u5bfc\u6211\u4e86\u89e3\u8fd9\u4e2a\u6a21\u578b\u4ee5\u53ca\u5982\u4f55\u4f7f\u7528\u5b83\uff1f\u8bf7\u7528\u7b80\u5355\u6613\u61c2\u7684\u8bed\u8a00\u5411\u9ad8\u4e2d\u751f\u89e3\u91ca\u3002"</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="n">
+        <v>28705</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"""
+Create an G{n,m} random graph with n nodes and m edges
+and report some properties.
+This graph is sometimes called the Erd##[m~Qs-Rnyi graph
+but is different from G{n,p} or binomial_graph which is also
+sometimes called the Erd##[m~Qs-Rnyi graph.
+"""
+__author__ = """Aric Hagberg (hagberg@lanl.gov)"""
+__credits__ = """"""
+#    Copyright (C) 2004-2006 by 
+#    Aric Hagberg 
+#    Dan Schult 
+#    Pieter Swart 
+#    Distributed under the terms of the GNU Lesser General Public License
+#    http://www.gnu.org/copyleft/lesser.html
+from networkx import *
+import sys
+n=10 # 10 nodes
+m=20 # 20 edges
+G=gnm_random_graph(n,m)
+# some properties
+print "node degree clustering"
+for v in nodes(G):
+    print v,degree(G,v),clustering(G,v)
+# print the adjacency list to terminal 
+write_adjlist(G,sys.stdout)
+</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import torch.onnx
+import torchvision.models as models
+# 
+model = models.resnet18(pretrained=True)
+# 
+model.eval()
+# 
+x = torch.randn(1, 3, 224, 224)
+# 
+torch.onnx.export(model, x, "resnet18.onnx")
+import onnxruntime
+#  ONNX 
+session = onnxruntime.InferenceSession("resnet18.onnx")
+# 
+input_name = session.get_inputs()[0].name
+output_name = session.get_outputs()[0].name
+# 
+x = np.random.randn(1, 3, 224, 224).astype(np.float32)
+# 
+result = session.run([output_name], {input_name: x})
+</t>
+        </is>
+      </c>
+      <c r="J39" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>2</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>"\u90a3\u4ed6\u4eec\u548ctorch tensorflow\u7684\u533a\u522b\u5728\u54ea\u91cc\u5462"</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>"I need to be able to manipulate a large (10^7 nodes) graph in python. The data corresponding to each node/edge is minimal, say, a small number of strings. What is the most efficient, in terms of memory and speed, way of doing this? 
+A dict of dicts is more flexible and simpler to implement, but I intuitively expect a list of lists to be faster. The list option would also require that I keep the data separate from the structure, while dicts would allow for something of the sort:
+graph[I][J]["Property"]="value"
+What would you suggest?
+Yes, I should have been a bit clearer on what I mean by efficiency. In this particular case I mean it in terms of random access retrieval.
+Loading the data in to memory isn't a huge problem. That's done once and for all. The time consuming part is visiting the nodes so I can extract the information and measure the metrics I'm interested in.
+I hadn't considered making each node a class (properties are the same for all nodes) but it seems like that would add an extra layer of overhead? I was hoping someone would have some direct experience with a similar case that they could share. After all, graphs are one of the most common abstractions in CS.
+"</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>3</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>"\u4ed6\u4eec\u90fd\u662f\u56fe\u7ed3\u6784\u7684\u5417"</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>